<commit_message>
Reporte con fecha en nombre de archivo
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoAgentes.xlsx
+++ b/reportes/base/ocatalogoAgentes.xlsx
@@ -5,22 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4003299a955809c3/Escritorio/calera/reportes/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_A3AD8052060DDFB58B4CFB36282AC21238724DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2BA8810-DE52-4AD6-A3A0-3B5ADC10C03D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B56EC5-A762-40E4-A8B3-89C2F1DEDE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Catálogo de agentes de ventas.</t>
   </si>
@@ -39,12 +51,15 @@
   <si>
     <t>Correo</t>
   </si>
+  <si>
+    <t>Fecha:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +115,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aparajita"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -148,6 +169,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -155,7 +179,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -472,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,41 +519,46 @@
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11">
+        <f ca="1">TODAY()</f>
+        <v>44780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
@@ -534,7 +566,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
@@ -734,10 +766,16 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
+    <row r="41" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reporte Comprobante de pagos por venta
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoAgentes.xlsx
+++ b/reportes/base/ocatalogoAgentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E08E49-7E57-4869-AC40-5CE5F6DD8DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163DE0B7-DBD6-4A1E-AB28-B4270A085B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="21580" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +121,13 @@
       <color theme="1"/>
       <name val="Aparajita"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -175,6 +182,9 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -182,8 +192,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +512,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,21 +523,21 @@
     <col min="4" max="4" width="36.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="7">
         <f ca="1">TODAY()</f>
-        <v>44780</v>
+        <v>44785</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -535,16 +545,16 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -554,7 +564,7 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
@@ -773,14 +783,15 @@
       <c r="D41" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial Black,Normal"&amp;K00-048Minerales San Antonio SA de CV</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial Black,Normal"&amp;K00-046MINERALES SAN ANTONIO S.A. DE C.V.</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Datos de cliente en el reporte de agentes
</commit_message>
<xml_diff>
--- a/reportes/base/ocatalogoAgentes.xlsx
+++ b/reportes/base/ocatalogoAgentes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163DE0B7-DBD6-4A1E-AB28-B4270A085B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08F8D2F-90E1-4724-9BE2-0604C2DA7B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Catálogo de agentes de ventas.</t>
   </si>
   <si>
     <t>AGENTE</t>
-  </si>
-  <si>
-    <t>Nombre cliente</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -54,12 +51,15 @@
   <si>
     <t>Fecha:</t>
   </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +98,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Aparajita"/>
       <family val="1"/>
     </font>
@@ -138,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -150,6 +142,43 @@
       <left style="hair">
         <color indexed="64"/>
       </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="hair">
         <color indexed="64"/>
       </right>
@@ -168,32 +197,36 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,284 +542,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.36328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="B1" s="9"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="E2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6">
         <f ca="1">TODAY()</f>
-        <v>44785</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>